<commit_message>
improve excel format(columnn title)
</commit_message>
<xml_diff>
--- a/bookbag/testing/test.xlsx
+++ b/bookbag/testing/test.xlsx
@@ -9,6 +9,10 @@
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="部分">工作表1!$A:$A</definedName>
+    <definedName name="题号">工作表1!$B:$B</definedName>
+  </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -19,54 +23,70 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+  <si>
+    <t>单选</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
   <si>
     <t>I</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>单选</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>I</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>II</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>II</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>是非</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>多选</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>1,3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>填空</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>李白,杜甫</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>填空</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>部分</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>题号</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>类型</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>选项个数</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>答案</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -76,8 +96,17 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0_ "/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="宋体"/>
@@ -113,10 +142,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="普通" xfId="0" builtinId="0"/>
@@ -448,10 +486,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -463,83 +501,100 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1">
-        <v>4</v>
-      </c>
-      <c r="E1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>11</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>0</v>
+      </c>
+      <c r="D2" s="1">
+        <v>4</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="1">
-        <v>3</v>
-      </c>
       <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="1">
         <v>4</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" s="1">
-        <v>1</v>
-      </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D4" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B5" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D5" s="1">
         <v>2</v>
       </c>
+      <c r="E5" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="1">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="1">
+        <v>2</v>
+      </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>